<commit_message>
Mejora visual de Compra monedas y excel horas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golro\Documents\Universidad\año 3\primer cuatrimestre\IngenieriaDelSoftware\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB7B344-C4A6-4FD9-A17E-61204E13605D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430015C7-F1B2-4D08-9AC5-AF03D32FC1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -727,15 +727,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,10 +735,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -755,6 +742,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -775,6 +765,16 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,23 +1404,23 @@
   </sheetPr>
   <dimension ref="A2:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="147" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K61" sqref="K61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.87890625" customWidth="1"/>
-    <col min="3" max="3" width="48.64453125" customWidth="1"/>
-    <col min="5" max="5" width="13.87890625" customWidth="1"/>
-    <col min="7" max="7" width="53.3515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.1171875" customWidth="1"/>
-    <col min="11" max="11" width="35.41015625" customWidth="1"/>
-    <col min="12" max="12" width="26.87890625" customWidth="1"/>
-    <col min="16" max="16" width="17.41015625" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1"/>
+    <col min="7" max="7" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.109375" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.88671875" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1459,43 +1459,43 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>205.67</v>
+        <v>206.17</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="30"/>
-      <c r="K3" s="45">
+      <c r="K3" s="40">
         <f>F6+F12+F22+F21+F51+F52+F53+F61+F62+F63+F64</f>
         <v>48.5</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="37" t="s">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="39"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="36"/>
       <c r="J4" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="45"/>
-    </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="40"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="42"/>
+      <c r="K4" s="40"/>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
       <c r="J5" s="32"/>
-      <c r="K5" s="45"/>
+      <c r="K5" s="40"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1510,18 +1510,18 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="43">
         <f>F7+F13+F20+F43+F45+F46</f>
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1536,13 +1536,13 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="34"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="43"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
@@ -1557,13 +1557,13 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="34"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="43"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -1578,17 +1578,17 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="34">
+      <c r="K9" s="43">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F54+F55+F60+F65</f>
         <v>43.820000000000007</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1603,10 +1603,10 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="34"/>
-    </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J10" s="45"/>
+      <c r="K10" s="43"/>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1621,12 +1621,12 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="34"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="43"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>8</v>
       </c>
@@ -1641,15 +1641,15 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="34">
+      <c r="K12" s="43">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F47+F66+F67</f>
         <v>36.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
@@ -1664,10 +1664,10 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="51"/>
-      <c r="K13" s="34"/>
-    </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J13" s="47"/>
+      <c r="K13" s="43"/>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>11</v>
       </c>
@@ -1682,10 +1682,10 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J14" s="47"/>
+      <c r="K14" s="43"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1700,15 +1700,15 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="52" t="s">
+      <c r="J15" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="34">
+      <c r="K15" s="43">
         <f>F10+F16+F39+F40+F48+F49+F50</f>
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -1723,10 +1723,10 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="34"/>
-    </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J16" s="49"/>
+      <c r="K16" s="43"/>
+    </row>
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
@@ -1741,10 +1741,10 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="34"/>
-    </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="J17" s="49"/>
+      <c r="K17" s="43"/>
+    </row>
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
@@ -1761,15 +1761,15 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="34">
+      <c r="K18" s="43">
         <f>F11+F23+F25+F27+F29+F31+F56+F57+F58+F59+F68+F69</f>
         <v>17.25</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>11</v>
       </c>
@@ -1787,10 +1787,10 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="36"/>
-      <c r="K19" s="34"/>
-    </row>
-    <row r="20" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="J19" s="51"/>
+      <c r="K19" s="43"/>
+    </row>
+    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
@@ -1807,10 +1807,10 @@
         <v>20</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="J20" s="36"/>
-      <c r="K20" s="34"/>
-    </row>
-    <row r="21" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="J20" s="51"/>
+      <c r="K20" s="43"/>
+    </row>
+    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
@@ -1828,7 +1828,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>8</v>
       </c>
@@ -1845,13 +1845,13 @@
         <v>5</v>
       </c>
       <c r="G22" s="11"/>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="44"/>
-      <c r="L22" s="44"/>
-    </row>
-    <row r="23" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+    </row>
+    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="G23" s="11"/>
     </row>
-    <row r="24" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>11</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1921,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -1937,7 +1937,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>11</v>
       </c>
@@ -1955,7 +1955,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2006,7 +2006,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2038,7 +2038,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2146,7 +2146,7 @@
       </c>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2164,25 +2164,25 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
-      <c r="B41" s="37" t="s">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B41" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="39"/>
-    </row>
-    <row r="42" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
-      <c r="B42" s="40"/>
-      <c r="C42" s="41"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="41"/>
-      <c r="G42" s="42"/>
-    </row>
-    <row r="43" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="36"/>
+    </row>
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B42" s="37"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="39"/>
+    </row>
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>10</v>
       </c>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>10</v>
       </c>
@@ -2232,7 +2232,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
@@ -2245,10 +2245,12 @@
       <c r="E46" s="1">
         <v>3</v>
       </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-    </row>
-    <row r="47" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+      <c r="F46" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2266,7 +2268,7 @@
       </c>
       <c r="G47" s="11"/>
     </row>
-    <row r="48" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>15</v>
       </c>
@@ -2284,7 +2286,7 @@
       </c>
       <c r="G48" s="29"/>
     </row>
-    <row r="49" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -2302,7 +2304,7 @@
       </c>
       <c r="G49" s="29"/>
     </row>
-    <row r="50" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -2320,7 +2322,7 @@
       </c>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>8</v>
       </c>
@@ -2338,7 +2340,7 @@
       </c>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -2356,7 +2358,7 @@
       </c>
       <c r="G52" s="7"/>
     </row>
-    <row r="53" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>8</v>
       </c>
@@ -2374,7 +2376,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>11</v>
       </c>
@@ -2390,7 +2392,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>11</v>
       </c>
@@ -2408,7 +2410,7 @@
       </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>16</v>
       </c>
@@ -2426,7 +2428,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -2442,7 +2444,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -2460,7 +2462,7 @@
       </c>
       <c r="G58" s="11"/>
     </row>
-    <row r="59" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -2476,7 +2478,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>11</v>
       </c>
@@ -2492,7 +2494,7 @@
       </c>
       <c r="G60" s="11"/>
     </row>
-    <row r="61" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>8</v>
       </c>
@@ -2510,7 +2512,7 @@
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>8</v>
       </c>
@@ -2528,7 +2530,7 @@
       </c>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>8</v>
       </c>
@@ -2546,7 +2548,7 @@
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>8</v>
       </c>
@@ -2564,7 +2566,7 @@
       </c>
       <c r="G64" s="11"/>
     </row>
-    <row r="65" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
         <v>11</v>
       </c>
@@ -2583,7 +2585,7 @@
       </c>
       <c r="G65" s="11"/>
     </row>
-    <row r="66" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="8" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2601,7 @@
       </c>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
@@ -2611,7 +2613,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
         <v>16</v>
       </c>
@@ -2629,7 +2631,7 @@
       </c>
       <c r="G68" s="7"/>
     </row>
-    <row r="69" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>16</v>
       </c>
@@ -2676,21 +2678,21 @@
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.64453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.64453125" customWidth="1"/>
-    <col min="2" max="2" width="35.41015625" customWidth="1"/>
-    <col min="3" max="3" width="27.234375" customWidth="1"/>
-    <col min="4" max="4" width="10.234375" customWidth="1"/>
-    <col min="7" max="7" width="17.41015625" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>55</v>
       </c>
@@ -2717,10 +2719,10 @@
       </c>
       <c r="K1" s="2">
         <f>SUM(B2:B1000)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -2749,7 +2751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -2770,7 +2772,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -2793,7 +2795,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -2806,7 +2808,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -2827,7 +2829,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -2848,7 +2850,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -2861,7 +2863,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -2882,7 +2884,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -2895,7 +2897,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -2908,7 +2910,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -2921,7 +2923,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -2934,7 +2936,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -2947,7 +2949,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -2960,7 +2962,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -2973,7 +2975,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -2986,7 +2988,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -3007,7 +3009,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -3028,7 +3030,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -3041,7 +3043,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -3062,7 +3064,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -3075,7 +3077,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -3088,7 +3090,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -3122,7 +3124,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -3143,7 +3145,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -3156,7 +3158,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -3179,7 +3181,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -3192,7 +3194,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -3205,7 +3207,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -3228,7 +3230,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -3270,7 +3272,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -3291,7 +3293,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -3304,7 +3306,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -3317,7 +3319,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -3338,7 +3340,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -3351,7 +3353,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -3364,7 +3366,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -3385,7 +3387,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -3406,7 +3408,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -3427,11 +3429,13 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
-      <c r="B43" s="19"/>
+      <c r="B43" s="17">
+        <v>1</v>
+      </c>
       <c r="C43" s="16" t="s">
         <v>104</v>
       </c>
@@ -3448,7 +3452,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -3471,7 +3475,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -3492,7 +3496,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -3505,7 +3509,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -3526,7 +3530,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Excel estadisticas semana 2
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5B9F21-C4C5-4EBF-8806-0B35DF9D6F56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498FD759-746B-42AB-8907-22B664A7C29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="123">
   <si>
     <t>Nombre</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>Animación moneda ventana dinero</t>
+  </si>
+  <si>
+    <t>DEMO3</t>
+  </si>
+  <si>
+    <t>Semana 2</t>
+  </si>
+  <si>
+    <t>Horas trabajadas</t>
+  </si>
+  <si>
+    <t>Horas estimadas</t>
   </si>
 </sst>
 </file>
@@ -475,7 +487,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -544,24 +556,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -576,6 +570,48 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -706,34 +742,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="8" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="13" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -742,6 +757,27 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -790,8 +826,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1419,10 +1453,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P70"/>
+  <dimension ref="A2:P73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="65" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1479,35 +1513,35 @@
         <v>207.86999999999998</v>
       </c>
       <c r="G3" s="1"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="40">
+      <c r="J3" s="23"/>
+      <c r="K3" s="42">
         <f>F6+F12+F22+F21+F51+F52+F53+F61+F62+F63+F64+F70</f>
         <v>49.2</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="J4" s="31" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
+      <c r="J4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="40"/>
+      <c r="K4" s="42"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="37"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="39"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="40"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="41"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="42"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
@@ -1527,10 +1561,10 @@
         <v>6</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="J6" s="41" t="s">
+      <c r="J6" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="43">
+      <c r="K6" s="45">
         <f>F7+F13+F20+F43+F45+F46</f>
         <v>31.5</v>
       </c>
@@ -1553,8 +1587,8 @@
         <v>4</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="43"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="45"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
@@ -1574,8 +1608,8 @@
         <v>4.5</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="43"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="45"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
@@ -1595,10 +1629,10 @@
         <v>5</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="43">
+      <c r="K9" s="45">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F54+F55+F60+F65</f>
         <v>43.820000000000007</v>
       </c>
@@ -1620,8 +1654,8 @@
         <v>3</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="43"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="45"/>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
@@ -1638,8 +1672,8 @@
         <v>1.5</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="43"/>
+      <c r="J11" s="47"/>
+      <c r="K11" s="45"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
@@ -1658,10 +1692,10 @@
         <v>3</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="J12" s="46" t="s">
+      <c r="J12" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="43">
+      <c r="K12" s="45">
         <f>F9+F15+F32+F33+F34+F35+F36+F37+F38+F47+F66+F67</f>
         <v>36.6</v>
       </c>
@@ -1681,8 +1715,8 @@
         <v>2.5</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="J13" s="47"/>
-      <c r="K13" s="43"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="45"/>
     </row>
     <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -1699,8 +1733,8 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="J14" s="47"/>
-      <c r="K14" s="43"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="45"/>
     </row>
     <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
@@ -1717,10 +1751,10 @@
         <v>1.5</v>
       </c>
       <c r="G15" s="7"/>
-      <c r="J15" s="48" t="s">
+      <c r="J15" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="K15" s="43">
+      <c r="K15" s="45">
         <f>F10+F16+F39+F40+F48+F49+F50</f>
         <v>27</v>
       </c>
@@ -1740,8 +1774,8 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="43"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="45"/>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
@@ -1758,8 +1792,8 @@
         <v>0.5</v>
       </c>
       <c r="G17" s="7"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="43"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="45"/>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
@@ -1778,10 +1812,10 @@
         <v>2</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="J18" s="50" t="s">
+      <c r="J18" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="43">
+      <c r="K18" s="45">
         <f>F11+F23+F25+F27+F29+F31+F56+F57+F58+F59+F68+F69</f>
         <v>17.25</v>
       </c>
@@ -1804,8 +1838,8 @@
         <v>1.5</v>
       </c>
       <c r="G19" s="7"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="43"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="45"/>
     </row>
     <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
@@ -1824,8 +1858,8 @@
         <v>20</v>
       </c>
       <c r="G20" s="11"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="43"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="45"/>
     </row>
     <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
@@ -1861,12 +1895,12 @@
       <c r="F22" s="1">
         <v>5</v>
       </c>
-      <c r="G22" s="11"/>
-      <c r="J22" s="52" t="s">
+      <c r="G22" s="7"/>
+      <c r="J22" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="K22" s="53"/>
-      <c r="L22" s="53"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="55"/>
     </row>
     <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
@@ -1884,7 +1918,7 @@
       <c r="F23" s="1">
         <v>0.5</v>
       </c>
-      <c r="G23" s="11"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -2047,7 +2081,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2059,9 +2093,9 @@
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="55"/>
-    </row>
-    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G33" s="28"/>
+    </row>
+    <row r="34" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2079,7 +2113,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2097,7 +2131,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2115,7 +2149,7 @@
       </c>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2125,7 +2159,7 @@
       <c r="D37" s="1">
         <v>33</v>
       </c>
-      <c r="E37" s="33">
+      <c r="E37" s="26">
         <v>1.5</v>
       </c>
       <c r="F37" s="1">
@@ -2133,7 +2167,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2151,7 +2185,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2169,7 +2203,7 @@
       </c>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2187,25 +2221,25 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="34" t="s">
+    <row r="41" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B41" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
-      <c r="F41" s="35"/>
-      <c r="G41" s="36"/>
-    </row>
-    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="39"/>
-    </row>
-    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="37"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="38"/>
+    </row>
+    <row r="42" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="B42" s="39"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="41"/>
+    </row>
+    <row r="43" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>10</v>
       </c>
@@ -2223,7 +2257,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>11</v>
       </c>
@@ -2241,7 +2275,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>10</v>
       </c>
@@ -2259,7 +2293,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
@@ -2276,8 +2310,17 @@
         <v>1.5</v>
       </c>
       <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I46" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="J46" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="K46" s="35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
@@ -2294,8 +2337,19 @@
         <v>4</v>
       </c>
       <c r="G47" s="11"/>
-    </row>
-    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I47" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47">
+        <f>F52+F51+F61+F62+F63+F64+F70+5.5</f>
+        <v>11.7</v>
+      </c>
+      <c r="K47">
+        <f>E52+E51+E61+E62+E63+E64+E70</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
         <v>15</v>
       </c>
@@ -2311,9 +2365,20 @@
       <c r="F48" s="1">
         <v>6</v>
       </c>
-      <c r="G48" s="29"/>
-    </row>
-    <row r="49" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G48" s="22"/>
+      <c r="I48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48">
+        <f>F44+F54+F55+F60+F65+15</f>
+        <v>29.6</v>
+      </c>
+      <c r="K48">
+        <f>E44+E54+E55+E60+E65</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -2329,9 +2394,20 @@
       <c r="F49" s="1">
         <v>4.5</v>
       </c>
-      <c r="G49" s="29"/>
-    </row>
-    <row r="50" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="G49" s="22"/>
+      <c r="I49" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J49">
+        <f>F56+F57+F58+F59+F68+F69</f>
+        <v>11.2</v>
+      </c>
+      <c r="K49">
+        <f>E56+E57+E58+E59+E68+E69</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -2348,8 +2424,19 @@
         <v>1</v>
       </c>
       <c r="G50" s="7"/>
-    </row>
-    <row r="51" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J50">
+        <f>F48+F49+F50</f>
+        <v>11.5</v>
+      </c>
+      <c r="K50">
+        <f>E48+E49+E50</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="4" t="s">
         <v>8</v>
       </c>
@@ -2366,8 +2453,19 @@
         <v>0.5</v>
       </c>
       <c r="G51" s="7"/>
-    </row>
-    <row r="52" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J51">
+        <f>F43+F45+F46+5</f>
+        <v>10</v>
+      </c>
+      <c r="K51">
+        <f>E43+E45+E46</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>8</v>
       </c>
@@ -2384,8 +2482,19 @@
         <v>1</v>
       </c>
       <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="I52" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <f>F66+F47</f>
+        <v>7</v>
+      </c>
+      <c r="K52">
+        <f>E66+E47</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>8</v>
       </c>
@@ -2403,7 +2512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>11</v>
       </c>
@@ -2419,7 +2528,7 @@
       </c>
       <c r="G54" s="11"/>
     </row>
-    <row r="55" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>11</v>
       </c>
@@ -2437,7 +2546,7 @@
       </c>
       <c r="G55" s="11"/>
     </row>
-    <row r="56" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="10" t="s">
         <v>16</v>
       </c>
@@ -2455,7 +2564,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -2473,7 +2582,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -2491,7 +2600,7 @@
       </c>
       <c r="G58" s="7"/>
     </row>
-    <row r="59" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -2507,7 +2616,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="6" t="s">
         <v>11</v>
       </c>
@@ -2523,7 +2632,7 @@
       </c>
       <c r="G60" s="7"/>
     </row>
-    <row r="61" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="4" t="s">
         <v>8</v>
       </c>
@@ -2541,7 +2650,7 @@
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>8</v>
       </c>
@@ -2559,7 +2668,7 @@
       </c>
       <c r="G62" s="7"/>
     </row>
-    <row r="63" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>8</v>
       </c>
@@ -2577,7 +2686,7 @@
       </c>
       <c r="G63" s="7"/>
     </row>
-    <row r="64" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>8</v>
       </c>
@@ -2642,7 +2751,7 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="55"/>
+      <c r="G67" s="28"/>
     </row>
     <row r="68" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="10" t="s">
@@ -2698,8 +2807,33 @@
       </c>
       <c r="G70" s="7"/>
     </row>
+    <row r="71" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="38"/>
+    </row>
+    <row r="72" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="39"/>
+      <c r="C72" s="40"/>
+      <c r="D72" s="40"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="41"/>
+    </row>
+    <row r="73" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="B71:G72"/>
     <mergeCell ref="B41:G42"/>
     <mergeCell ref="K3:K5"/>
     <mergeCell ref="J6:J8"/>
@@ -2727,8 +2861,8 @@
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2790,7 +2924,7 @@
       <c r="F2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="18">
+      <c r="G2" s="30">
         <v>45202</v>
       </c>
       <c r="J2" s="12" t="s">
@@ -2804,7 +2938,7 @@
       <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="18"/>
       <c r="C3" s="16" t="s">
         <v>67</v>
       </c>
@@ -2814,10 +2948,10 @@
       <c r="E3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="21">
+      <c r="G3" s="31">
         <v>45202</v>
       </c>
     </row>
@@ -2837,10 +2971,10 @@
       <c r="E4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="31">
         <v>45202</v>
       </c>
     </row>
@@ -2848,12 +2982,14 @@
       <c r="A5" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="16" t="s">
         <v>69</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
@@ -2861,7 +2997,7 @@
       <c r="A6" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="22"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="16" t="s">
         <v>70</v>
       </c>
@@ -2874,9 +3010,7 @@
       <c r="F6" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="23">
-        <v>45216</v>
-      </c>
+      <c r="G6" s="29"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
@@ -2897,7 +3031,7 @@
       <c r="F7" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -2905,12 +3039,14 @@
       <c r="A8" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="16" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
+      <c r="E8" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
@@ -2918,7 +3054,7 @@
       <c r="A9" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="16" t="s">
         <v>42</v>
       </c>
@@ -2931,7 +3067,7 @@
       <c r="F9" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -2939,12 +3075,14 @@
       <c r="A10" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="16" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="E10" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
@@ -2952,12 +3090,14 @@
       <c r="A11" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="19"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="16" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
+      <c r="E11" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
@@ -2965,12 +3105,14 @@
       <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="19"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="16" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+      <c r="E12" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
@@ -2978,12 +3120,14 @@
       <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="19"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="16" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
@@ -2991,12 +3135,14 @@
       <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="16" t="s">
         <v>79</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
@@ -3004,12 +3150,14 @@
       <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="19"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="16" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
@@ -3017,12 +3165,14 @@
       <c r="A16" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="19"/>
+      <c r="B16" s="18"/>
       <c r="C16" s="16" t="s">
         <v>81</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
@@ -3030,12 +3180,14 @@
       <c r="A17" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="19"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="16" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
@@ -3043,7 +3195,7 @@
       <c r="A18" s="15">
         <v>17</v>
       </c>
-      <c r="B18" s="19"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="16" t="s">
         <v>83</v>
       </c>
@@ -3053,10 +3205,10 @@
       <c r="E18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3064,7 +3216,7 @@
       <c r="A19" s="15">
         <v>18</v>
       </c>
-      <c r="B19" s="19"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="16" t="s">
         <v>26</v>
       </c>
@@ -3074,10 +3226,10 @@
       <c r="E19" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3085,12 +3237,14 @@
       <c r="A20" s="15">
         <v>19</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="16" t="s">
         <v>84</v>
       </c>
       <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
@@ -3098,7 +3252,7 @@
       <c r="A21" s="15">
         <v>20</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="16" t="s">
         <v>34</v>
       </c>
@@ -3108,10 +3262,10 @@
       <c r="E21" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3119,12 +3273,14 @@
       <c r="A22" s="15">
         <v>21</v>
       </c>
-      <c r="B22" s="19"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="16" t="s">
         <v>85</v>
       </c>
       <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
@@ -3132,12 +3288,14 @@
       <c r="A23" s="15">
         <v>22</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="16" t="s">
         <v>86</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
@@ -3145,7 +3303,7 @@
       <c r="A24" s="15">
         <v>23</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="16" t="s">
         <v>87</v>
       </c>
@@ -3158,7 +3316,7 @@
       <c r="F24" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3166,12 +3324,14 @@
       <c r="A25" s="15">
         <v>24</v>
       </c>
-      <c r="B25" s="19"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="16" t="s">
         <v>88</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
@@ -3179,7 +3339,7 @@
       <c r="A26" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="16" t="s">
         <v>20</v>
       </c>
@@ -3189,10 +3349,10 @@
       <c r="E26" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3200,12 +3360,14 @@
       <c r="A27" s="15">
         <v>26</v>
       </c>
-      <c r="B27" s="19"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
@@ -3228,7 +3390,7 @@
       <c r="F28" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="31">
         <v>45202</v>
       </c>
     </row>
@@ -3236,12 +3398,14 @@
       <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="19"/>
+      <c r="B29" s="18"/>
       <c r="C29" s="16" t="s">
         <v>91</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
@@ -3249,12 +3413,14 @@
       <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="19"/>
+      <c r="B30" s="18"/>
       <c r="C30" s="16" t="s">
         <v>92</v>
       </c>
       <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
@@ -3274,10 +3440,10 @@
       <c r="E31" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="31">
         <v>45202</v>
       </c>
     </row>
@@ -3285,7 +3451,7 @@
       <c r="A32" s="15">
         <v>31</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="18"/>
       <c r="C32" s="16" t="s">
         <v>94</v>
       </c>
@@ -3295,10 +3461,10 @@
       <c r="E32" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3306,7 +3472,7 @@
       <c r="A33" s="15">
         <v>32</v>
       </c>
-      <c r="B33" s="24"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="16" t="s">
         <v>95</v>
       </c>
@@ -3316,10 +3482,10 @@
       <c r="E33" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3327,7 +3493,7 @@
       <c r="A34" s="15">
         <v>33</v>
       </c>
-      <c r="B34" s="19"/>
+      <c r="B34" s="18"/>
       <c r="C34" s="16" t="s">
         <v>32</v>
       </c>
@@ -3337,10 +3503,10 @@
       <c r="E34" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3348,12 +3514,14 @@
       <c r="A35" s="15">
         <v>34</v>
       </c>
-      <c r="B35" s="19"/>
+      <c r="B35" s="18"/>
       <c r="C35" s="16" t="s">
         <v>96</v>
       </c>
       <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
+      <c r="E35" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
@@ -3361,12 +3529,14 @@
       <c r="A36" s="15">
         <v>35</v>
       </c>
-      <c r="B36" s="19"/>
+      <c r="B36" s="18"/>
       <c r="C36" s="16" t="s">
         <v>97</v>
       </c>
       <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
+      <c r="E36" s="13" t="s">
+        <v>74</v>
+      </c>
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
@@ -3374,7 +3544,7 @@
       <c r="A37" s="15">
         <v>36</v>
       </c>
-      <c r="B37" s="19"/>
+      <c r="B37" s="18"/>
       <c r="C37" s="16" t="s">
         <v>45</v>
       </c>
@@ -3387,7 +3557,7 @@
       <c r="F37" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G37" s="26">
+      <c r="G37" s="32">
         <v>45216</v>
       </c>
     </row>
@@ -3395,12 +3565,14 @@
       <c r="A38" s="15">
         <v>37</v>
       </c>
-      <c r="B38" s="19"/>
+      <c r="B38" s="18"/>
       <c r="C38" s="16" t="s">
         <v>98</v>
       </c>
       <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
+      <c r="E38" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
@@ -3408,12 +3580,14 @@
       <c r="A39" s="15">
         <v>38</v>
       </c>
-      <c r="B39" s="19"/>
+      <c r="B39" s="18"/>
       <c r="C39" s="16" t="s">
         <v>99</v>
       </c>
       <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
+      <c r="E39" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
@@ -3421,7 +3595,7 @@
       <c r="A40" s="15">
         <v>39</v>
       </c>
-      <c r="B40" s="19"/>
+      <c r="B40" s="18"/>
       <c r="C40" s="16" t="s">
         <v>100</v>
       </c>
@@ -3434,7 +3608,7 @@
       <c r="F40" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3442,7 +3616,7 @@
       <c r="A41" s="15">
         <v>40</v>
       </c>
-      <c r="B41" s="19"/>
+      <c r="B41" s="18"/>
       <c r="C41" s="16" t="s">
         <v>102</v>
       </c>
@@ -3455,7 +3629,7 @@
       <c r="F41" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="G41" s="25">
+      <c r="G41" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3463,7 +3637,7 @@
       <c r="A42" s="15">
         <v>41</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="18"/>
       <c r="C42" s="16" t="s">
         <v>103</v>
       </c>
@@ -3476,7 +3650,7 @@
       <c r="F42" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3484,7 +3658,7 @@
       <c r="A43" s="15">
         <v>42</v>
       </c>
-      <c r="B43" s="54"/>
+      <c r="B43" s="27"/>
       <c r="C43" s="16" t="s">
         <v>104</v>
       </c>
@@ -3497,7 +3671,7 @@
       <c r="F43" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3517,10 +3691,10 @@
       <c r="E44" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G44" s="25">
+      <c r="G44" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3528,7 +3702,7 @@
       <c r="A45" s="15">
         <v>44</v>
       </c>
-      <c r="B45" s="24"/>
+      <c r="B45" s="21"/>
       <c r="C45" s="16" t="s">
         <v>106</v>
       </c>
@@ -3541,7 +3715,7 @@
       <c r="F45" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G45" s="25">
+      <c r="G45" s="34">
         <v>45216</v>
       </c>
     </row>
@@ -3549,12 +3723,14 @@
       <c r="A46" s="15">
         <v>45</v>
       </c>
-      <c r="B46" s="19"/>
+      <c r="B46" s="18"/>
       <c r="C46" s="16" t="s">
         <v>107</v>
       </c>
       <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
+      <c r="E46" s="13" t="s">
+        <v>101</v>
+      </c>
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
@@ -3575,7 +3751,7 @@
       <c r="F47" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="G47" s="27">
+      <c r="G47" s="33">
         <v>45216</v>
       </c>
     </row>
@@ -3596,7 +3772,7 @@
       <c r="F48" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G48" s="28">
+      <c r="G48" s="33">
         <v>45216</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sombras y correccion de bug
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golro\Documents\Universidad\año 3\primer cuatrimestre\IngenieriaDelSoftware\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315FD10-AFF9-46A4-B618-F17A16A9AC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928351ED-1976-4A12-AA30-5ABB0515411F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -1547,23 +1547,23 @@
   </sheetPr>
   <dimension ref="A2:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" zoomScale="111" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K79" sqref="K79"/>
+    <sheetView tabSelected="1" topLeftCell="G69" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.52734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.8203125" customWidth="1"/>
-    <col min="3" max="3" width="48.52734375" customWidth="1"/>
-    <col min="5" max="5" width="13.8203125" customWidth="1"/>
-    <col min="7" max="7" width="53.46875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.17578125" customWidth="1"/>
-    <col min="11" max="11" width="35.46875" customWidth="1"/>
-    <col min="12" max="12" width="26.8203125" customWidth="1"/>
-    <col min="16" max="16" width="17.46875" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="3" max="3" width="48.5546875" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" customWidth="1"/>
+    <col min="11" max="11" width="35.44140625" customWidth="1"/>
+    <col min="12" max="12" width="26.77734375" customWidth="1"/>
+    <col min="16" max="16" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1598,11 +1598,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E992)</f>
-        <v>174.5</v>
+        <v>178.5</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>215.36999999999998</v>
+        <v>223.76999999999995</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="23"/>
@@ -1611,7 +1611,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1625,7 @@
       </c>
       <c r="K4" s="44"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -1638,7 +1638,7 @@
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
     </row>
-    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1664,7 +1664,7 @@
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
     </row>
-    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1685,7 +1685,7 @@
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1706,7 +1706,7 @@
       <c r="M8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="J10" s="47"/>
       <c r="K10" s="46"/>
     </row>
-    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
     </row>
-    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1810,7 @@
       <c r="J13" s="48"/>
       <c r="K13" s="46"/>
     </row>
-    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>13</v>
       </c>
@@ -1828,7 +1828,7 @@
       <c r="J14" s="48"/>
       <c r="K14" s="46"/>
     </row>
-    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>14</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>15</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="J16" s="49"/>
       <c r="K16" s="46"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>16</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="J17" s="49"/>
       <c r="K17" s="46"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>16</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>23.25</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>13</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="J19" s="50"/>
       <c r="K19" s="46"/>
     </row>
-    <row r="20" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1953,7 +1953,7 @@
       <c r="J20" s="50"/>
       <c r="K20" s="46"/>
     </row>
-    <row r="21" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -1994,7 +1994,7 @@
       <c r="K22" s="51"/>
       <c r="L22" s="51"/>
     </row>
-    <row r="23" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2048,7 +2048,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2084,7 +2084,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2155,7 +2155,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2187,7 +2187,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="27"/>
     </row>
-    <row r="34" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2277,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B41" s="43" t="s">
         <v>36</v>
       </c>
@@ -2323,7 +2323,7 @@
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
     </row>
-    <row r="42" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -2331,7 +2331,7 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
     </row>
-    <row r="43" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2367,7 +2367,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -2385,7 +2385,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2403,7 +2403,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -2439,7 +2439,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -2656,7 +2656,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -2786,7 +2786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>9</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
         <v>9</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>9</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="G65" s="7"/>
     </row>
-    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="6" t="s">
         <v>13</v>
       </c>
@@ -2910,7 +2910,7 @@
       </c>
       <c r="G66" s="7"/>
     </row>
-    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
@@ -2928,7 +2928,7 @@
       </c>
       <c r="G67" s="7"/>
     </row>
-    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="8" t="s">
         <v>14</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="G68" s="27"/>
     </row>
-    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
         <v>16</v>
       </c>
@@ -2964,7 +2964,7 @@
       </c>
       <c r="G69" s="7"/>
     </row>
-    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="10" t="s">
         <v>16</v>
       </c>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="G70" s="7"/>
     </row>
-    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
@@ -3000,7 +3000,7 @@
       </c>
       <c r="G71" s="7"/>
     </row>
-    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="43" t="s">
         <v>67</v>
       </c>
@@ -3019,7 +3019,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="43"/>
       <c r="C73" s="43"/>
       <c r="D73" s="43"/>
@@ -3030,7 +3030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="4" t="s">
         <v>9</v>
       </c>
@@ -3050,10 +3050,14 @@
       </c>
       <c r="J74">
         <f>SUM(F91,F80)</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>9.9</v>
+      </c>
+      <c r="K74">
+        <f>SUM(E80,E91)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
         <v>12</v>
       </c>
@@ -3070,7 +3074,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
         <v>15</v>
       </c>
@@ -3087,7 +3091,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
         <v>15</v>
       </c>
@@ -3104,7 +3108,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="9" t="s">
         <v>15</v>
       </c>
@@ -3129,7 +3133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="10" t="s">
         <v>16</v>
       </c>
@@ -3143,9 +3147,9 @@
       <c r="F79" s="35">
         <v>4</v>
       </c>
-      <c r="G79" s="35"/>
-    </row>
-    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G79" s="11"/>
+    </row>
+    <row r="80" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>13</v>
       </c>
@@ -3157,11 +3161,11 @@
         <v>3</v>
       </c>
       <c r="F80" s="35">
-        <v>1.5</v>
+        <v>7.2</v>
       </c>
       <c r="G80" s="11"/>
     </row>
-    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
         <v>16</v>
       </c>
@@ -3175,7 +3179,7 @@
       <c r="F81" s="35"/>
       <c r="G81" s="35"/>
     </row>
-    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
         <v>16</v>
       </c>
@@ -3191,9 +3195,9 @@
       <c r="F82" s="35">
         <v>2</v>
       </c>
-      <c r="G82" s="35"/>
-    </row>
-    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G82" s="11"/>
+    </row>
+    <row r="83" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -3209,7 +3213,7 @@
       <c r="F83" s="35"/>
       <c r="G83" s="35"/>
     </row>
-    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
         <v>14</v>
       </c>
@@ -3223,7 +3227,7 @@
       <c r="F84" s="35"/>
       <c r="G84" s="35"/>
     </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -3237,7 +3241,7 @@
       <c r="F85" s="35"/>
       <c r="G85" s="35"/>
     </row>
-    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
         <v>14</v>
       </c>
@@ -3251,7 +3255,7 @@
       <c r="F86" s="35"/>
       <c r="G86" s="35"/>
     </row>
-    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="37" t="s">
         <v>14</v>
       </c>
@@ -3267,7 +3271,7 @@
       <c r="F87" s="38"/>
       <c r="G87" s="38"/>
     </row>
-    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9" t="s">
         <v>15</v>
       </c>
@@ -3279,7 +3283,7 @@
       <c r="F88" s="35"/>
       <c r="G88" s="35"/>
     </row>
-    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
         <v>12</v>
       </c>
@@ -3295,7 +3299,7 @@
       <c r="F89" s="35"/>
       <c r="G89" s="35"/>
     </row>
-    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
         <v>12</v>
       </c>
@@ -3311,7 +3315,7 @@
       <c r="F90" s="35"/>
       <c r="G90" s="35"/>
     </row>
-    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
         <v>13</v>
       </c>
@@ -3321,11 +3325,15 @@
       <c r="D91" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E91" s="35"/>
-      <c r="F91" s="35"/>
-      <c r="G91" s="35"/>
-    </row>
-    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E91" s="35">
+        <v>4</v>
+      </c>
+      <c r="F91" s="35">
+        <v>2.7</v>
+      </c>
+      <c r="G91" s="11"/>
+    </row>
+    <row r="92" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="4" t="s">
         <v>9</v>
       </c>
@@ -3341,7 +3349,7 @@
       <c r="F92" s="35"/>
       <c r="G92" s="35"/>
     </row>
-    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>9</v>
       </c>
@@ -3357,7 +3365,7 @@
       <c r="F93" s="35"/>
       <c r="G93" s="35"/>
     </row>
-    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -3373,7 +3381,7 @@
       <c r="F94" s="35"/>
       <c r="G94" s="35"/>
     </row>
-    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>9</v>
       </c>
@@ -3389,7 +3397,7 @@
       <c r="F95" s="35"/>
       <c r="G95" s="35"/>
     </row>
-    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="41" t="s">
         <v>15</v>
       </c>
@@ -3401,7 +3409,7 @@
       <c r="F96" s="38"/>
       <c r="G96" s="38"/>
     </row>
-    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="38" t="s">
         <v>146</v>
       </c>
@@ -3413,7 +3421,7 @@
       <c r="F97" s="38"/>
       <c r="G97" s="38"/>
     </row>
-    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>12</v>
       </c>
@@ -3460,17 +3468,17 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.52734375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.52734375" customWidth="1"/>
-    <col min="2" max="2" width="35.46875" customWidth="1"/>
-    <col min="3" max="3" width="27.17578125" customWidth="1"/>
-    <col min="4" max="4" width="10.17578125" customWidth="1"/>
-    <col min="7" max="7" width="17.46875" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>92</v>
       </c>
@@ -3500,7 +3508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>1</v>
       </c>
@@ -3529,7 +3537,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3550,7 +3558,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3573,7 +3581,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>4</v>
       </c>
@@ -3588,7 +3596,7 @@
       <c r="F5" s="13"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -3607,7 +3615,7 @@
       </c>
       <c r="G6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>6</v>
       </c>
@@ -3630,7 +3638,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>7</v>
       </c>
@@ -3645,7 +3653,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>8</v>
       </c>
@@ -3668,7 +3676,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <v>9</v>
       </c>
@@ -3683,7 +3691,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -3698,7 +3706,7 @@
       <c r="F11" s="13"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
@@ -3713,7 +3721,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <v>12</v>
       </c>
@@ -3728,7 +3736,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <v>13</v>
       </c>
@@ -3743,7 +3751,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <v>14</v>
       </c>
@@ -3758,7 +3766,7 @@
       <c r="F15" s="13"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
         <v>15</v>
       </c>
@@ -3773,7 +3781,7 @@
       <c r="F16" s="13"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>16</v>
       </c>
@@ -3788,7 +3796,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -3809,7 +3817,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -3830,7 +3838,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -3847,7 +3855,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -3868,7 +3876,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -3883,7 +3891,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -3898,7 +3906,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -3919,7 +3927,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -3934,7 +3942,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -3957,7 +3965,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -3972,7 +3980,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -3995,7 +4003,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -4010,7 +4018,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -4025,7 +4033,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -4048,7 +4056,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -4069,7 +4077,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -4090,7 +4098,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -4111,7 +4119,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -4126,7 +4134,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -4141,7 +4149,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -4164,7 +4172,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -4179,7 +4187,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -4194,7 +4202,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -4215,7 +4223,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -4236,7 +4244,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -4259,7 +4267,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -4282,7 +4290,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -4305,7 +4313,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -4326,7 +4334,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -4341,7 +4349,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="12.7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -4362,7 +4370,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>47</v>
       </c>
@@ -4385,7 +4393,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="39"/>
       <c r="C49" s="40"/>
     </row>
@@ -4395,23 +4403,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -4620,32 +4611,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4662,4 +4645,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
mejora x2 toolbar ayuda refractor
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928351ED-1976-4A12-AA30-5ABB0515411F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B5DD4-F093-42DE-B03E-A5B3BD3D3B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -506,10 +506,10 @@
     <t>Arrancar la aplicación por cmd en una máquina vacía</t>
   </si>
   <si>
-    <t>;Mejora Interfaz venta/compra monedas</t>
-  </si>
-  <si>
     <t>Demo 1</t>
+  </si>
+  <si>
+    <t>Mejora Interfaz venta/compra monedas</t>
   </si>
 </sst>
 </file>
@@ -1547,7 +1547,7 @@
   </sheetPr>
   <dimension ref="A2:P98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G69" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>223.76999999999995</v>
+        <v>225.56999999999996</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="23"/>
@@ -1725,8 +1725,8 @@
         <v>13</v>
       </c>
       <c r="K9" s="46">
-        <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66</f>
-        <v>43.820000000000007</v>
+        <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+F91+F80</f>
+        <v>55.52000000000001</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2390,7 +2390,7 @@
         <v>12</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D46" s="1">
         <v>47</v>
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G49" s="22"/>
       <c r="I49" s="34" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J49" s="34" t="s">
         <v>45</v>
@@ -3050,7 +3050,7 @@
       </c>
       <c r="J74">
         <f>SUM(F91,F80)</f>
-        <v>9.9</v>
+        <v>11.7</v>
       </c>
       <c r="K74">
         <f>SUM(E80,E91)</f>
@@ -3161,7 +3161,7 @@
         <v>3</v>
       </c>
       <c r="F80" s="35">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="G80" s="11"/>
     </row>
@@ -3329,7 +3329,7 @@
         <v>4</v>
       </c>
       <c r="F91" s="35">
-        <v>2.7</v>
+        <v>3.7</v>
       </c>
       <c r="G91" s="11"/>
     </row>
@@ -4403,6 +4403,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -4611,24 +4628,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4645,29 +4670,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Interfaz juegos de cartas + cartel cartal mas alta
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahdm\Workspace\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442B5DD4-F093-42DE-B03E-A5B3BD3D3B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544A747-425D-46ED-9961-71EA1EC11132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificador" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="156">
   <si>
     <t>Nombre</t>
   </si>
@@ -510,6 +510,21 @@
   </si>
   <si>
     <t>Mejora Interfaz venta/compra monedas</t>
+  </si>
+  <si>
+    <t>DEMO4</t>
+  </si>
+  <si>
+    <t>Hacer un juego multijugador (continuación)</t>
+  </si>
+  <si>
+    <t>Rediseñar interfaz de cartas</t>
+  </si>
+  <si>
+    <t>Animación ruleta europea</t>
+  </si>
+  <si>
+    <t>Retrasada a siguiente demo</t>
   </si>
 </sst>
 </file>
@@ -519,7 +534,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -593,6 +608,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="22">
@@ -723,7 +745,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -805,11 +827,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -902,6 +944,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1545,22 +1600,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P98"/>
+  <dimension ref="A2:P107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="3" max="3" width="48.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.21875" customWidth="1"/>
-    <col min="11" max="11" width="35.44140625" customWidth="1"/>
-    <col min="12" max="12" width="26.77734375" customWidth="1"/>
-    <col min="16" max="16" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="7" max="7" width="53.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.1796875" customWidth="1"/>
+    <col min="11" max="11" width="35.453125" customWidth="1"/>
+    <col min="12" max="12" width="26.81640625" customWidth="1"/>
+    <col min="16" max="16" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,7 +1644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1598,11 +1653,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E992)</f>
-        <v>178.5</v>
+        <v>206.5</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>225.56999999999996</v>
+        <v>228.06999999999996</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="23"/>
@@ -1611,7 +1666,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="43" t="s">
         <v>8</v>
       </c>
@@ -1625,7 +1680,7 @@
       </c>
       <c r="K4" s="44"/>
     </row>
-    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B5" s="43"/>
       <c r="C5" s="43"/>
       <c r="D5" s="43"/>
@@ -1933,7 +1988,7 @@
       <c r="J19" s="50"/>
       <c r="K19" s="46"/>
     </row>
-    <row r="20" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1953,7 +2008,7 @@
       <c r="J20" s="50"/>
       <c r="K20" s="46"/>
     </row>
-    <row r="21" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -1971,7 +2026,7 @@
       </c>
       <c r="G21" s="7"/>
     </row>
-    <row r="22" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
@@ -1994,7 +2049,7 @@
       <c r="K22" s="51"/>
       <c r="L22" s="51"/>
     </row>
-    <row r="23" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2012,7 +2067,7 @@
       </c>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>13</v>
       </c>
@@ -2030,7 +2085,7 @@
       </c>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2048,7 +2103,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>13</v>
       </c>
@@ -2066,7 +2121,7 @@
       </c>
       <c r="G26" s="11"/>
     </row>
-    <row r="27" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2084,7 +2139,7 @@
       </c>
       <c r="G27" s="11"/>
     </row>
-    <row r="28" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>13</v>
       </c>
@@ -2102,7 +2157,7 @@
       </c>
       <c r="G28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>16</v>
       </c>
@@ -2120,7 +2175,7 @@
       </c>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>13</v>
       </c>
@@ -2138,7 +2193,7 @@
       </c>
       <c r="G30" s="11"/>
     </row>
-    <row r="31" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
@@ -2155,7 +2210,7 @@
       <c r="G31" s="11"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B32" s="8" t="s">
         <v>14</v>
       </c>
@@ -2173,7 +2228,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B33" s="8" t="s">
         <v>14</v>
       </c>
@@ -2187,7 +2242,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="27"/>
     </row>
-    <row r="34" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B34" s="8" t="s">
         <v>14</v>
       </c>
@@ -2205,7 +2260,7 @@
       </c>
       <c r="G34" s="11"/>
     </row>
-    <row r="35" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B35" s="8" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2278,7 @@
       </c>
       <c r="G35" s="11"/>
     </row>
-    <row r="36" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B36" s="8" t="s">
         <v>14</v>
       </c>
@@ -2241,7 +2296,7 @@
       </c>
       <c r="G36" s="11"/>
     </row>
-    <row r="37" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
@@ -2259,7 +2314,7 @@
       </c>
       <c r="G37" s="7"/>
     </row>
-    <row r="38" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>14</v>
       </c>
@@ -2277,7 +2332,7 @@
       </c>
       <c r="G38" s="11"/>
     </row>
-    <row r="39" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
         <v>15</v>
       </c>
@@ -2295,7 +2350,7 @@
       </c>
       <c r="G39" s="11"/>
     </row>
-    <row r="40" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>15</v>
       </c>
@@ -2313,7 +2368,7 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B41" s="43" t="s">
         <v>36</v>
       </c>
@@ -2323,7 +2378,7 @@
       <c r="F41" s="43"/>
       <c r="G41" s="43"/>
     </row>
-    <row r="42" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B42" s="43"/>
       <c r="C42" s="43"/>
       <c r="D42" s="43"/>
@@ -2331,7 +2386,7 @@
       <c r="F42" s="43"/>
       <c r="G42" s="43"/>
     </row>
-    <row r="43" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
         <v>12</v>
       </c>
@@ -2349,7 +2404,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>13</v>
       </c>
@@ -2367,7 +2422,7 @@
       </c>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>12</v>
       </c>
@@ -2385,7 +2440,7 @@
       </c>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>12</v>
       </c>
@@ -2403,7 +2458,7 @@
       </c>
       <c r="G46" s="7"/>
     </row>
-    <row r="47" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>12</v>
       </c>
@@ -2421,7 +2476,7 @@
       </c>
       <c r="G47" s="7"/>
     </row>
-    <row r="48" spans="2:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B48" s="8" t="s">
         <v>14</v>
       </c>
@@ -2439,7 +2494,7 @@
       </c>
       <c r="G48" s="11"/>
     </row>
-    <row r="49" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="9" t="s">
         <v>15</v>
       </c>
@@ -2466,7 +2521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>15</v>
       </c>
@@ -2495,7 +2550,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>15</v>
       </c>
@@ -2524,7 +2579,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>9</v>
       </c>
@@ -2553,7 +2608,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>9</v>
       </c>
@@ -2582,7 +2637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>9</v>
       </c>
@@ -2611,7 +2666,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>13</v>
       </c>
@@ -2638,7 +2693,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>13</v>
       </c>
@@ -2656,7 +2711,7 @@
       </c>
       <c r="G56" s="11"/>
     </row>
-    <row r="57" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
         <v>16</v>
       </c>
@@ -2674,7 +2729,7 @@
       </c>
       <c r="G57" s="11"/>
     </row>
-    <row r="58" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B58" s="10" t="s">
         <v>16</v>
       </c>
@@ -2701,7 +2756,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B59" s="10" t="s">
         <v>16</v>
       </c>
@@ -2730,7 +2785,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
         <v>16</v>
       </c>
@@ -2759,7 +2814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
         <v>13</v>
       </c>
@@ -3044,7 +3099,9 @@
         <v>2</v>
       </c>
       <c r="F74" s="1"/>
-      <c r="G74" s="35"/>
+      <c r="G74" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="I74" s="6" t="s">
         <v>13</v>
       </c>
@@ -3069,7 +3126,9 @@
       </c>
       <c r="E75" s="35"/>
       <c r="F75" s="35"/>
-      <c r="G75" s="35"/>
+      <c r="G75" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="I75" s="9" t="s">
         <v>15</v>
       </c>
@@ -3086,7 +3145,9 @@
       </c>
       <c r="E76" s="35"/>
       <c r="F76" s="35"/>
-      <c r="G76" s="35"/>
+      <c r="G76" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="I76" s="5" t="s">
         <v>12</v>
       </c>
@@ -3103,7 +3164,9 @@
       </c>
       <c r="E77" s="35"/>
       <c r="F77" s="35"/>
-      <c r="G77" s="35"/>
+      <c r="G77" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="I77" s="8" t="s">
         <v>14</v>
       </c>
@@ -3120,7 +3183,9 @@
       </c>
       <c r="E78" s="35"/>
       <c r="F78" s="35"/>
-      <c r="G78" s="35"/>
+      <c r="G78" s="14" t="s">
+        <v>155</v>
+      </c>
       <c r="I78" s="10" t="s">
         <v>16</v>
       </c>
@@ -3177,7 +3242,9 @@
         <v>3</v>
       </c>
       <c r="F81" s="35"/>
-      <c r="G81" s="35"/>
+      <c r="G81" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="82" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="10" t="s">
@@ -3211,7 +3278,9 @@
         <v>1</v>
       </c>
       <c r="F83" s="35"/>
-      <c r="G83" s="35"/>
+      <c r="G83" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="84" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="8" t="s">
@@ -3225,9 +3294,11 @@
       </c>
       <c r="E84" s="35"/>
       <c r="F84" s="35"/>
-      <c r="G84" s="35"/>
-    </row>
-    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G84" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B85" s="8" t="s">
         <v>14</v>
       </c>
@@ -3239,7 +3310,9 @@
       </c>
       <c r="E85" s="35"/>
       <c r="F85" s="35"/>
-      <c r="G85" s="35"/>
+      <c r="G85" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="86" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="8" t="s">
@@ -3253,7 +3326,9 @@
       </c>
       <c r="E86" s="35"/>
       <c r="F86" s="35"/>
-      <c r="G86" s="35"/>
+      <c r="G86" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="87" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="37" t="s">
@@ -3269,7 +3344,9 @@
         <v>3</v>
       </c>
       <c r="F87" s="38"/>
-      <c r="G87" s="38"/>
+      <c r="G87" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="88" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9" t="s">
@@ -3281,7 +3358,9 @@
       <c r="D88" s="35"/>
       <c r="E88" s="35"/>
       <c r="F88" s="35"/>
-      <c r="G88" s="35"/>
+      <c r="G88" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="89" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
@@ -3297,7 +3376,9 @@
         <v>1</v>
       </c>
       <c r="F89" s="35"/>
-      <c r="G89" s="35"/>
+      <c r="G89" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="90" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
@@ -3313,7 +3394,9 @@
         <v>2</v>
       </c>
       <c r="F90" s="35"/>
-      <c r="G90" s="35"/>
+      <c r="G90" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="91" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="6" t="s">
@@ -3347,7 +3430,9 @@
         <v>4</v>
       </c>
       <c r="F92" s="35"/>
-      <c r="G92" s="35"/>
+      <c r="G92" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="93" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
@@ -3363,9 +3448,11 @@
         <v>1</v>
       </c>
       <c r="F93" s="35"/>
-      <c r="G93" s="35"/>
-    </row>
-    <row r="94" spans="2:7" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G93" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="94" spans="2:7" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="4" t="s">
         <v>9</v>
       </c>
@@ -3379,7 +3466,9 @@
         <v>1</v>
       </c>
       <c r="F94" s="35"/>
-      <c r="G94" s="35"/>
+      <c r="G94" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="95" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
@@ -3395,7 +3484,9 @@
         <v>2</v>
       </c>
       <c r="F95" s="35"/>
-      <c r="G95" s="35"/>
+      <c r="G95" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="96" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="41" t="s">
@@ -3407,7 +3498,9 @@
       <c r="D96" s="38"/>
       <c r="E96" s="38"/>
       <c r="F96" s="38"/>
-      <c r="G96" s="38"/>
+      <c r="G96" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="97" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="38" t="s">
@@ -3419,7 +3512,9 @@
       <c r="D97" s="38"/>
       <c r="E97" s="38"/>
       <c r="F97" s="38"/>
-      <c r="G97" s="38"/>
+      <c r="G97" s="14" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="98" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
@@ -3431,10 +3526,147 @@
       <c r="D98" s="35"/>
       <c r="E98" s="35"/>
       <c r="F98" s="35"/>
-      <c r="G98" s="35"/>
+      <c r="G98" s="14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="99" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="53" t="s">
+        <v>151</v>
+      </c>
+      <c r="C99" s="54"/>
+      <c r="D99" s="54"/>
+      <c r="E99" s="54"/>
+      <c r="F99" s="54"/>
+      <c r="G99" s="54"/>
+    </row>
+    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="55"/>
+      <c r="C100" s="56"/>
+      <c r="D100" s="56"/>
+      <c r="E100" s="56"/>
+      <c r="F100" s="56"/>
+      <c r="G100" s="56"/>
+    </row>
+    <row r="101" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D101" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" s="35">
+        <v>4</v>
+      </c>
+      <c r="F101" s="35"/>
+      <c r="G101" s="35"/>
+    </row>
+    <row r="102" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="D102" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="35">
+        <v>1</v>
+      </c>
+      <c r="F102" s="35">
+        <v>2</v>
+      </c>
+      <c r="G102" s="7"/>
+    </row>
+    <row r="103" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C103" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="D103" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="35">
+        <v>1</v>
+      </c>
+      <c r="F103" s="35"/>
+      <c r="G103" s="35"/>
+    </row>
+    <row r="104" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D104" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="35">
+        <v>2</v>
+      </c>
+      <c r="F104" s="35"/>
+      <c r="G104" s="35"/>
+    </row>
+    <row r="105" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C105" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="D105" s="35">
+        <v>24</v>
+      </c>
+      <c r="E105" s="35">
+        <v>15</v>
+      </c>
+      <c r="F105" s="35"/>
+      <c r="G105" s="35"/>
+    </row>
+    <row r="106" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" s="35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D106" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E106" s="35">
+        <v>3</v>
+      </c>
+      <c r="F106" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="G106" s="7"/>
+    </row>
+    <row r="107" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D107" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E107" s="35">
+        <v>2</v>
+      </c>
+      <c r="F107" s="35"/>
+      <c r="G107" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B99:G100"/>
     <mergeCell ref="B72:G73"/>
     <mergeCell ref="B41:G42"/>
     <mergeCell ref="K3:K5"/>
@@ -3468,13 +3700,13 @@
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3537,7 +3769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
         <v>2</v>
       </c>
@@ -3558,7 +3790,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>3</v>
       </c>
@@ -3796,7 +4028,7 @@
       <c r="F17" s="13"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
         <v>17</v>
       </c>
@@ -3817,7 +4049,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <v>18</v>
       </c>
@@ -3838,7 +4070,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>19</v>
       </c>
@@ -3855,7 +4087,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
         <v>20</v>
       </c>
@@ -3876,7 +4108,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>21</v>
       </c>
@@ -3891,7 +4123,7 @@
       <c r="F22" s="13"/>
       <c r="G22" s="15"/>
     </row>
-    <row r="23" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>22</v>
       </c>
@@ -3906,7 +4138,7 @@
       <c r="F23" s="13"/>
       <c r="G23" s="15"/>
     </row>
-    <row r="24" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>23</v>
       </c>
@@ -3927,7 +4159,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>24</v>
       </c>
@@ -3942,7 +4174,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="15"/>
     </row>
-    <row r="26" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
         <v>25</v>
       </c>
@@ -3965,7 +4197,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <v>26</v>
       </c>
@@ -3980,7 +4212,7 @@
       <c r="F27" s="13"/>
       <c r="G27" s="15"/>
     </row>
-    <row r="28" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <v>27</v>
       </c>
@@ -4003,7 +4235,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <v>28</v>
       </c>
@@ -4018,7 +4250,7 @@
       <c r="F29" s="13"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>29</v>
       </c>
@@ -4033,7 +4265,7 @@
       <c r="F30" s="13"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A31" s="15">
         <v>30</v>
       </c>
@@ -4056,7 +4288,7 @@
         <v>45202</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A32" s="15">
         <v>31</v>
       </c>
@@ -4077,7 +4309,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A33" s="15">
         <v>32</v>
       </c>
@@ -4098,7 +4330,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A34" s="15">
         <v>33</v>
       </c>
@@ -4119,7 +4351,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>34</v>
       </c>
@@ -4134,7 +4366,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="15"/>
     </row>
-    <row r="36" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>35</v>
       </c>
@@ -4149,7 +4381,7 @@
       <c r="F36" s="13"/>
       <c r="G36" s="15"/>
     </row>
-    <row r="37" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -4172,7 +4404,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -4187,7 +4419,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="15"/>
     </row>
-    <row r="39" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -4202,7 +4434,7 @@
       <c r="F39" s="13"/>
       <c r="G39" s="15"/>
     </row>
-    <row r="40" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>39</v>
       </c>
@@ -4223,7 +4455,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>40</v>
       </c>
@@ -4244,7 +4476,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A42" s="15">
         <v>41</v>
       </c>
@@ -4267,7 +4499,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A43" s="15">
         <v>42</v>
       </c>
@@ -4290,7 +4522,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="14" x14ac:dyDescent="0.3">
       <c r="A44" s="15">
         <v>43</v>
       </c>
@@ -4313,7 +4545,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A45" s="15">
         <v>44</v>
       </c>
@@ -4334,7 +4566,7 @@
         <v>45216</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>45</v>
       </c>
@@ -4349,7 +4581,7 @@
       <c r="F46" s="13"/>
       <c r="G46" s="15"/>
     </row>
-    <row r="47" spans="1:7" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="12.5" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>46</v>
       </c>
@@ -4403,23 +4635,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -4628,32 +4843,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4670,4 +4877,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
alerta de reglas cartas
</commit_message>
<xml_diff>
--- a/Documentación/To Do - Requisitos_ 2ª Version.xlsx
+++ b/Documentación/To Do - Requisitos_ 2ª Version.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34616\Desktop\CEU\tercer año\primer_semestre\ing_software\Konguitos_Casino\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF58C1CF-B9CC-4B64-BE66-347842DB683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A398CAEB-6428-4FAC-B3DC-0CF29ACCFBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="153">
   <si>
     <t>Nombre</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>herencia html toolbar</t>
+  </si>
+  <si>
+    <t>Ajustes (pt. 2)</t>
   </si>
 </sst>
 </file>
@@ -1548,10 +1551,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:P99"/>
+  <dimension ref="A2:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:K14"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="83" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1601,11 +1604,11 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1">
         <f t="shared" ref="E3:F3" si="0">SUM(E6:E992)</f>
-        <v>179.5</v>
+        <v>181.5</v>
       </c>
       <c r="F3" s="3">
         <f t="shared" si="0"/>
-        <v>226.56999999999996</v>
+        <v>228.46999999999994</v>
       </c>
       <c r="G3" s="1"/>
       <c r="J3" s="23"/>
@@ -1729,7 +1732,7 @@
       </c>
       <c r="K9" s="46">
         <f>F8+F14+F19+F24+F26+F28+F30+F44+F55+F56+F61+F66+F91+F80+F99</f>
-        <v>56.52000000000001</v>
+        <v>58.420000000000009</v>
       </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
@@ -2137,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="F30" s="1">
-        <v>22.17</v>
+        <v>23.57</v>
       </c>
       <c r="G30" s="11"/>
     </row>
@@ -2520,7 +2523,7 @@
       </c>
       <c r="J51">
         <f>F14+F24+F26+F28+F30+F8-15.17</f>
-        <v>12.550000000000002</v>
+        <v>13.950000000000001</v>
       </c>
       <c r="K51">
         <f>E8+E19+E24+E26+E28+E30</f>
@@ -3053,7 +3056,7 @@
       </c>
       <c r="J74">
         <f>SUM(F91+F80+F99)</f>
-        <v>12.7</v>
+        <v>13.2</v>
       </c>
       <c r="K74">
         <f>SUM(E80+E91+E99)</f>
@@ -3164,7 +3167,7 @@
         <v>3</v>
       </c>
       <c r="F80" s="35">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G80" s="11"/>
     </row>
@@ -3450,7 +3453,23 @@
       <c r="F99" s="35">
         <v>1</v>
       </c>
-      <c r="G99" s="11"/>
+      <c r="G99" s="7"/>
+    </row>
+    <row r="100" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D100" s="1">
+        <v>39</v>
+      </c>
+      <c r="E100" s="1">
+        <v>2</v>
+      </c>
+      <c r="F100" s="1"/>
+      <c r="G100" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -3483,14 +3502,14 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="39.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.21875" customWidth="1"/>
     <col min="4" max="4" width="10.21875" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" customWidth="1"/>
@@ -4422,6 +4441,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002ACE3BD3BD6E0C4C9762278BB0DF607B" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="fab7ba1af23be20b30c2a2672ed67a22">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf" xmlns:ns4="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="531abb56a789977dee09b3cb67363cc8" ns3:_="" ns4:_="">
     <xsd:import namespace="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
@@ -4630,24 +4666,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
+    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="6940eef6-fc62-4b65-9bd8-c66fd5d892a7" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B364D9CE-BB59-43E7-813A-8F81412AF980}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4664,29 +4708,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9686506-EA07-42D8-AD05-D46E593ADF62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DF5F28B-5105-40F9-976F-62D07B763C33}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6940eef6-fc62-4b65-9bd8-c66fd5d892a7"/>
-    <ds:schemaRef ds:uri="b93fd186-45b2-483c-a5e2-2f5c4e9c14cf"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>